<commit_message>
Added file read feature
</commit_message>
<xml_diff>
--- a/src/main/java/com/company/resources/Matrix.xlsx
+++ b/src/main/java/com/company/resources/Matrix.xlsx
@@ -121,7 +121,7 @@
       <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="n">
@@ -172,13 +172,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="n">
@@ -190,6 +190,9 @@
       <c r="C1" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="D1" s="0" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
@@ -201,6 +204,9 @@
       <c r="C2" s="0" t="n">
         <v>6</v>
       </c>
+      <c r="D2" s="0" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
@@ -210,6 +216,9 @@
         <v>8</v>
       </c>
       <c r="C3" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="D3" s="0" t="n">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added write into file feature
</commit_message>
<xml_diff>
--- a/src/main/java/com/company/resources/Matrix.xlsx
+++ b/src/main/java/com/company/resources/Matrix.xlsx
@@ -5,16 +5,16 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Лист2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1"/>
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
@@ -25,7 +25,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -48,6 +48,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Mangal"/>
+      <family val="2"/>
       <charset val="204"/>
     </font>
   </fonts>
@@ -68,7 +75,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -92,6 +99,9 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -99,18 +109,85 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Comma" xfId="15" builtinId="3"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Заголовок" xfId="20"/>
   </cellStyles>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B1" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C1" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D1" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -118,80 +195,20 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="n">
-        <v>23</v>
-      </c>
-      <c r="B1" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="C1" s="0" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="B2" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="C2" s="0" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C3" s="0" t="n">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Обычный"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Обычный"&amp;12Страница &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C1" s="0" t="n">
         <v>3</v>
-      </c>
-      <c r="D1" s="0" t="n">
-        <v>5</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -204,9 +221,6 @@
       <c r="C2" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="D2" s="0" t="n">
-        <v>7</v>
-      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
@@ -218,17 +232,14 @@
       <c r="C3" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="D3" s="0" t="n">
-        <v>9</v>
-      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Обычный"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Обычный"&amp;12Страница &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>